<commit_message>
Add XMP put/get on the K computer
</commit_message>
<xml_diff>
--- a/data/K.xlsx
+++ b/data/K.xlsx
@@ -4,13 +4,15 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="25317"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="7560" yWindow="0" windowWidth="25600" windowHeight="14440" tabRatio="500"/>
+    <workbookView xWindow="4800" yWindow="460" windowWidth="25600" windowHeight="16060" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Summary" sheetId="2" r:id="rId1"/>
     <sheet name="SendRecv" sheetId="1" r:id="rId2"/>
-    <sheet name="K_PUT" sheetId="4" r:id="rId3"/>
-    <sheet name="K_GET" sheetId="5" r:id="rId4"/>
+    <sheet name="FUJITSU_PUT" sheetId="4" r:id="rId3"/>
+    <sheet name="FUJITSU_GET" sheetId="5" r:id="rId4"/>
+    <sheet name="XMP_PUT" sheetId="6" r:id="rId5"/>
+    <sheet name="XMP_GET" sheetId="7" r:id="rId6"/>
   </sheets>
   <calcPr calcId="140000" concurrentCalc="0"/>
   <extLst>
@@ -22,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="12">
   <si>
     <t>MAX（MB/s)</t>
     <phoneticPr fontId="1"/>
@@ -51,11 +53,53 @@
     <t>K-1.2.0-15</t>
   </si>
   <si>
-    <t>K_PUT</t>
+    <t>Fujitsu_PUT</t>
     <phoneticPr fontId="1"/>
   </si>
   <si>
-    <t>K_GET</t>
+    <t>Fujitsu_GET</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>XMP_PUT</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>XMP_GET</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>PUT/GETの性能差の理由は、Fujitsu_put/getは静的に領域を確保しているのに対し、XMP_put/getは（コンパイラが暗黙的に）動的に領域を確保しているから</t>
+    <rPh sb="8" eb="11">
+      <t>セイノウサ</t>
+    </rPh>
+    <rPh sb="12" eb="14">
+      <t>リユウ</t>
+    </rPh>
+    <rPh sb="32" eb="34">
+      <t>セイテキ</t>
+    </rPh>
+    <rPh sb="35" eb="37">
+      <t>リョウイキ</t>
+    </rPh>
+    <rPh sb="38" eb="40">
+      <t>カクホ</t>
+    </rPh>
+    <rPh sb="46" eb="47">
+      <t>タイ</t>
+    </rPh>
+    <rPh sb="68" eb="71">
+      <t>アンモクテキ</t>
+    </rPh>
+    <rPh sb="73" eb="75">
+      <t>ドウテキ</t>
+    </rPh>
+    <rPh sb="76" eb="78">
+      <t>リョウイキ</t>
+    </rPh>
+    <rPh sb="79" eb="81">
+      <t>カクホ</t>
+    </rPh>
     <phoneticPr fontId="1"/>
   </si>
 </sst>
@@ -115,8 +159,18 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="27">
+  <cellStyleXfs count="37">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -147,7 +201,7 @@
   <cellXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
   </cellXfs>
-  <cellStyles count="27">
+  <cellStyles count="37">
     <cellStyle name="ハイパーリンク" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="ハイパーリンク" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="ハイパーリンク" xfId="5" builtinId="8" hidden="1"/>
@@ -161,6 +215,11 @@
     <cellStyle name="ハイパーリンク" xfId="21" builtinId="8" hidden="1"/>
     <cellStyle name="ハイパーリンク" xfId="23" builtinId="8" hidden="1"/>
     <cellStyle name="ハイパーリンク" xfId="25" builtinId="8" hidden="1"/>
+    <cellStyle name="ハイパーリンク" xfId="27" builtinId="8" hidden="1"/>
+    <cellStyle name="ハイパーリンク" xfId="29" builtinId="8" hidden="1"/>
+    <cellStyle name="ハイパーリンク" xfId="31" builtinId="8" hidden="1"/>
+    <cellStyle name="ハイパーリンク" xfId="33" builtinId="8" hidden="1"/>
+    <cellStyle name="ハイパーリンク" xfId="35" builtinId="8" hidden="1"/>
     <cellStyle name="標準" xfId="0" builtinId="0"/>
     <cellStyle name="表示済みのハイパーリンク" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="表示済みのハイパーリンク" xfId="4" builtinId="9" hidden="1"/>
@@ -175,6 +234,11 @@
     <cellStyle name="表示済みのハイパーリンク" xfId="22" builtinId="9" hidden="1"/>
     <cellStyle name="表示済みのハイパーリンク" xfId="24" builtinId="9" hidden="1"/>
     <cellStyle name="表示済みのハイパーリンク" xfId="26" builtinId="9" hidden="1"/>
+    <cellStyle name="表示済みのハイパーリンク" xfId="28" builtinId="9" hidden="1"/>
+    <cellStyle name="表示済みのハイパーリンク" xfId="30" builtinId="9" hidden="1"/>
+    <cellStyle name="表示済みのハイパーリンク" xfId="32" builtinId="9" hidden="1"/>
+    <cellStyle name="表示済みのハイパーリンク" xfId="34" builtinId="9" hidden="1"/>
+    <cellStyle name="表示済みのハイパーリンク" xfId="36" builtinId="9" hidden="1"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleMedium4"/>
@@ -403,7 +467,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>K_PUT</c:v>
+                  <c:v>Fujitsu_PUT</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -510,67 +574,67 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="21"/>
                 <c:pt idx="0">
-                  <c:v>7.302602</c:v>
+                  <c:v>7.44879</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>14.103129</c:v>
+                  <c:v>14.375562</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>28.393966</c:v>
+                  <c:v>28.764045</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>43.671102</c:v>
+                  <c:v>44.107512</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>79.975008</c:v>
+                  <c:v>96.859629</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>153.846154</c:v>
+                  <c:v>172.043011</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>284.681679</c:v>
+                  <c:v>317.51938</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>483.817623</c:v>
+                  <c:v>521.916412</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>764.464352</c:v>
+                  <c:v>814.314115</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>1309.253636</c:v>
+                  <c:v>1392.013594</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>2063.995969</c:v>
+                  <c:v>2151.260504</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>2878.678731</c:v>
+                  <c:v>2965.161524</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>3589.833479</c:v>
+                  <c:v>3652.454996</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>4093.058114</c:v>
+                  <c:v>4133.98095</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>4402.525863</c:v>
+                  <c:v>4426.164185</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>4575.018761</c:v>
+                  <c:v>4587.869825</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>4666.019953</c:v>
+                  <c:v>4673.152601</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>4713.781586</c:v>
+                  <c:v>4716.919852</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>4737.784766</c:v>
+                  <c:v>4739.358685</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>4749.845987</c:v>
+                  <c:v>4750.548046</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>4755.952234</c:v>
+                  <c:v>4756.16526</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -586,7 +650,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>K_GET</c:v>
+                  <c:v>Fujitsu_GET</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -758,6 +822,326 @@
           </c:yVal>
           <c:smooth val="0"/>
         </c:ser>
+        <c:ser>
+          <c:idx val="3"/>
+          <c:order val="3"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Summary!$E$4</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>XMP_PUT</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Summary!$A$8:$A$28</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="21"/>
+                <c:pt idx="0">
+                  <c:v>8.0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>16.0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>32.0</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>64.0</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>128.0</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>256.0</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>512.0</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>1024.0</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>2048.0</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>4096.0</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>8192.0</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>16384.0</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>32768.0</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>65536.0</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>131072.0</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>262144.0</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>524288.0</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>1.048576E6</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>2.097152E6</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>4.194304E6</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>8.388608E6</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Summary!$E$8:$E$28</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="21"/>
+                <c:pt idx="0">
+                  <c:v>7.165249</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>13.769363</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>27.280477</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>41.898527</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>80.91024</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>153.661465</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>279.475983</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>482.563619</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>748.674831</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>1275.813736</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>1994.157741</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>2795.904437</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>3492.087174</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>3997.925881</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>4314.275369</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>4492.228601</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>4586.665734</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>4636.280633</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>4661.684487</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>4674.509332000001</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>4680.956089</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:ser>
+          <c:idx val="4"/>
+          <c:order val="4"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Summary!$F$4</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>XMP_GET</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Summary!$A$8:$A$28</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="21"/>
+                <c:pt idx="0">
+                  <c:v>8.0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>16.0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>32.0</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>64.0</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>128.0</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>256.0</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>512.0</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>1024.0</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>2048.0</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>4096.0</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>8192.0</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>16384.0</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>32768.0</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>65536.0</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>131072.0</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>262144.0</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>524288.0</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>1.048576E6</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>2.097152E6</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>4.194304E6</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>8.388608E6</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Summary!$F$8:$F$28</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="21"/>
+                <c:pt idx="0">
+                  <c:v>1.432921</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2.978129</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>5.986904000000001</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>11.962617</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>24.162341</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>47.132468</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>94.247584</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>184.089888</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>350.835118</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>663.319838</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>1168.782993</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>1876.961851</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>2690.753818</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>3437.954098</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>3993.479884</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>4343.476352</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>4541.21662</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>4649.251895</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>4704.191294</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>4732.852973</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>4746.854475</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+        </c:ser>
         <c:dLbls>
           <c:showLegendKey val="0"/>
           <c:showVal val="0"/>
@@ -766,11 +1150,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="2124983672"/>
-        <c:axId val="2124986472"/>
+        <c:axId val="2109582760"/>
+        <c:axId val="2109580632"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="2124983672"/>
+        <c:axId val="2109582760"/>
         <c:scaling>
           <c:logBase val="2.0"/>
           <c:orientation val="minMax"/>
@@ -794,13 +1178,13 @@
             <a:endParaRPr lang="ja-JP"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="2124986472"/>
+        <c:crossAx val="2109580632"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
         <c:majorUnit val="8.0"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="2124986472"/>
+        <c:axId val="2109580632"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="5000.0"/>
@@ -824,7 +1208,7 @@
             <a:endParaRPr lang="ja-JP"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="2124983672"/>
+        <c:crossAx val="2109582760"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
         <c:majorUnit val="1000.0"/>
@@ -838,8 +1222,8 @@
           <c:yMode val="edge"/>
           <c:x val="0.108853686471009"/>
           <c:y val="0.0901646829030092"/>
-          <c:w val="0.193249248389406"/>
-          <c:h val="0.209288408716352"/>
+          <c:w val="0.163970078740157"/>
+          <c:h val="0.348814014527254"/>
         </c:manualLayout>
       </c:layout>
       <c:overlay val="0"/>
@@ -1235,15 +1619,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D28"/>
+  <dimension ref="A1:G29"/>
   <sheetViews>
     <sheetView tabSelected="1" showRuler="0" topLeftCell="A2" workbookViewId="0">
-      <selection activeCell="F16" sqref="F16"/>
+      <selection activeCell="G30" sqref="G30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="12" defaultRowHeight="18" x14ac:dyDescent="0"/>
   <sheetData>
-    <row r="1" spans="1:4">
+    <row r="1" spans="1:6">
       <c r="A1" t="s">
         <v>5</v>
       </c>
@@ -1251,12 +1635,12 @@
         <v>6</v>
       </c>
     </row>
-    <row r="3" spans="1:4">
+    <row r="3" spans="1:6">
       <c r="B3" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="4" spans="1:4">
+    <row r="4" spans="1:6">
       <c r="A4" t="s">
         <v>2</v>
       </c>
@@ -1269,8 +1653,14 @@
       <c r="D4" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="5" spans="1:4">
+      <c r="E4" t="s">
+        <v>9</v>
+      </c>
+      <c r="F4" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6">
       <c r="A5">
         <v>1</v>
       </c>
@@ -1279,7 +1669,7 @@
         <v>0.69468600000000003</v>
       </c>
     </row>
-    <row r="6" spans="1:4">
+    <row r="6" spans="1:6">
       <c r="A6">
         <v>2</v>
       </c>
@@ -1288,7 +1678,7 @@
         <v>1.402525</v>
       </c>
     </row>
-    <row r="7" spans="1:4">
+    <row r="7" spans="1:6">
       <c r="A7">
         <v>4</v>
       </c>
@@ -1297,15 +1687,23 @@
         <v>2.7894000000000001</v>
       </c>
       <c r="C7">
-        <f>K_PUT!B2</f>
-        <v>3.5987399999999998</v>
+        <f>FUJITSU_PUT!B2</f>
+        <v>3.664682</v>
       </c>
       <c r="D7">
-        <f>K_GET!B2</f>
+        <f>FUJITSU_GET!B2</f>
         <v>0.733541</v>
       </c>
-    </row>
-    <row r="8" spans="1:4">
+      <c r="E7">
+        <f>XMP_PUT!B2</f>
+        <v>3.5366930000000001</v>
+      </c>
+      <c r="F7">
+        <f>XMP_GET!B2</f>
+        <v>0.72833199999999998</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6">
       <c r="A8">
         <v>8</v>
       </c>
@@ -1314,15 +1712,23 @@
         <v>5.5768559999999994</v>
       </c>
       <c r="C8">
-        <f>K_PUT!B3</f>
-        <v>7.3026020000000003</v>
+        <f>FUJITSU_PUT!B3</f>
+        <v>7.4487899999999998</v>
       </c>
       <c r="D8">
-        <f>K_GET!B3</f>
+        <f>FUJITSU_GET!B3</f>
         <v>1.443001</v>
       </c>
-    </row>
-    <row r="9" spans="1:4">
+      <c r="E8">
+        <f>XMP_PUT!B3</f>
+        <v>7.1652490000000002</v>
+      </c>
+      <c r="F8">
+        <f>XMP_GET!B3</f>
+        <v>1.4329210000000001</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6">
       <c r="A9">
         <v>16</v>
       </c>
@@ -1331,15 +1737,23 @@
         <v>11.138183000000001</v>
       </c>
       <c r="C9">
-        <f>K_PUT!B4</f>
-        <v>14.103129000000001</v>
+        <f>FUJITSU_PUT!B4</f>
+        <v>14.375562</v>
       </c>
       <c r="D9">
-        <f>K_GET!B4</f>
+        <f>FUJITSU_GET!B4</f>
         <v>3.0052590000000001</v>
       </c>
-    </row>
-    <row r="10" spans="1:4">
+      <c r="E9">
+        <f>XMP_PUT!B4</f>
+        <v>13.769363</v>
+      </c>
+      <c r="F9">
+        <f>XMP_GET!B4</f>
+        <v>2.978129</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6">
       <c r="A10">
         <v>32</v>
       </c>
@@ -1348,15 +1762,23 @@
         <v>17.650303000000001</v>
       </c>
       <c r="C10">
-        <f>K_PUT!B5</f>
-        <v>28.393965999999999</v>
+        <f>FUJITSU_PUT!B5</f>
+        <v>28.764044999999999</v>
       </c>
       <c r="D10">
-        <f>K_GET!B5</f>
+        <f>FUJITSU_GET!B5</f>
         <v>6.0457209999999995</v>
       </c>
-    </row>
-    <row r="11" spans="1:4">
+      <c r="E10">
+        <f>XMP_PUT!B5</f>
+        <v>27.280476999999998</v>
+      </c>
+      <c r="F10">
+        <f>XMP_GET!B5</f>
+        <v>5.9869040000000009</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6">
       <c r="A11">
         <v>64</v>
       </c>
@@ -1365,15 +1787,23 @@
         <v>35.155177000000002</v>
       </c>
       <c r="C11">
-        <f>K_PUT!B6</f>
-        <v>43.671101999999998</v>
+        <f>FUJITSU_PUT!B6</f>
+        <v>44.107512</v>
       </c>
       <c r="D11">
-        <f>K_GET!B6</f>
+        <f>FUJITSU_GET!B6</f>
         <v>12.070917</v>
       </c>
-    </row>
-    <row r="12" spans="1:4">
+      <c r="E11">
+        <f>XMP_PUT!B6</f>
+        <v>41.898527000000001</v>
+      </c>
+      <c r="F11">
+        <f>XMP_GET!B6</f>
+        <v>11.962617</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6">
       <c r="A12">
         <v>128</v>
       </c>
@@ -1382,15 +1812,23 @@
         <v>31.434185000000003</v>
       </c>
       <c r="C12">
-        <f>K_PUT!B7</f>
-        <v>79.975008000000003</v>
+        <f>FUJITSU_PUT!B7</f>
+        <v>96.859628999999998</v>
       </c>
       <c r="D12">
-        <f>K_GET!B7</f>
+        <f>FUJITSU_GET!B7</f>
         <v>23.811738000000002</v>
       </c>
-    </row>
-    <row r="13" spans="1:4">
+      <c r="E12">
+        <f>XMP_PUT!B7</f>
+        <v>80.910240000000002</v>
+      </c>
+      <c r="F12">
+        <f>XMP_GET!B7</f>
+        <v>24.162341000000001</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6">
       <c r="A13">
         <v>256</v>
       </c>
@@ -1399,15 +1837,23 @@
         <v>61.156235000000002</v>
       </c>
       <c r="C13">
-        <f>K_PUT!B8</f>
-        <v>153.84615400000001</v>
+        <f>FUJITSU_PUT!B8</f>
+        <v>172.04301100000001</v>
       </c>
       <c r="D13">
-        <f>K_GET!B8</f>
+        <f>FUJITSU_GET!B8</f>
         <v>46.813569000000001</v>
       </c>
-    </row>
-    <row r="14" spans="1:4">
+      <c r="E13">
+        <f>XMP_PUT!B8</f>
+        <v>153.66146499999999</v>
+      </c>
+      <c r="F13">
+        <f>XMP_GET!B8</f>
+        <v>47.132468000000003</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6">
       <c r="A14">
         <v>512</v>
       </c>
@@ -1416,15 +1862,23 @@
         <v>113.77777800000001</v>
       </c>
       <c r="C14">
-        <f>K_PUT!B9</f>
-        <v>284.68167900000003</v>
+        <f>FUJITSU_PUT!B9</f>
+        <v>317.51938000000001</v>
       </c>
       <c r="D14">
-        <f>K_GET!B9</f>
+        <f>FUJITSU_GET!B9</f>
         <v>93.592907000000011</v>
       </c>
-    </row>
-    <row r="15" spans="1:4">
+      <c r="E14">
+        <f>XMP_PUT!B9</f>
+        <v>279.47598299999999</v>
+      </c>
+      <c r="F14">
+        <f>XMP_GET!B9</f>
+        <v>94.247584000000003</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6">
       <c r="A15">
         <v>1024</v>
       </c>
@@ -1433,15 +1887,23 @@
         <v>207.91878199999999</v>
       </c>
       <c r="C15">
-        <f>K_PUT!B10</f>
-        <v>483.81762300000003</v>
+        <f>FUJITSU_PUT!B10</f>
+        <v>521.91641200000004</v>
       </c>
       <c r="D15">
-        <f>K_GET!B10</f>
+        <f>FUJITSU_GET!B10</f>
         <v>183.28262000000001</v>
       </c>
-    </row>
-    <row r="16" spans="1:4">
+      <c r="E15">
+        <f>XMP_PUT!B10</f>
+        <v>482.56361900000002</v>
+      </c>
+      <c r="F15">
+        <f>XMP_GET!B10</f>
+        <v>184.089888</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6">
       <c r="A16">
         <v>2048</v>
       </c>
@@ -1450,15 +1912,23 @@
         <v>339.15707500000002</v>
       </c>
       <c r="C16">
-        <f>K_PUT!B11</f>
-        <v>764.46435199999996</v>
+        <f>FUJITSU_PUT!B11</f>
+        <v>814.31411500000002</v>
       </c>
       <c r="D16">
-        <f>K_GET!B11</f>
+        <f>FUJITSU_GET!B11</f>
         <v>348.744146</v>
       </c>
-    </row>
-    <row r="17" spans="1:4">
+      <c r="E16">
+        <f>XMP_PUT!B11</f>
+        <v>748.67483100000004</v>
+      </c>
+      <c r="F16">
+        <f>XMP_GET!B11</f>
+        <v>350.83511800000002</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7">
       <c r="A17">
         <v>4096</v>
       </c>
@@ -1467,15 +1937,23 @@
         <v>567.43090700000005</v>
       </c>
       <c r="C17">
-        <f>K_PUT!B12</f>
-        <v>1309.2536359999999</v>
+        <f>FUJITSU_PUT!B12</f>
+        <v>1392.013594</v>
       </c>
       <c r="D17">
-        <f>K_GET!B12</f>
+        <f>FUJITSU_GET!B12</f>
         <v>653.63440500000002</v>
       </c>
-    </row>
-    <row r="18" spans="1:4">
+      <c r="E17">
+        <f>XMP_PUT!B12</f>
+        <v>1275.8137360000001</v>
+      </c>
+      <c r="F17">
+        <f>XMP_GET!B12</f>
+        <v>663.319838</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7">
       <c r="A18">
         <v>8192</v>
       </c>
@@ -1484,15 +1962,23 @@
         <v>847.72597900000005</v>
       </c>
       <c r="C18">
-        <f>K_PUT!B13</f>
-        <v>2063.9959690000001</v>
+        <f>FUJITSU_PUT!B13</f>
+        <v>2151.2605040000003</v>
       </c>
       <c r="D18">
-        <f>K_GET!B13</f>
+        <f>FUJITSU_GET!B13</f>
         <v>1151.3703439999999</v>
       </c>
-    </row>
-    <row r="19" spans="1:4">
+      <c r="E18">
+        <f>XMP_PUT!B13</f>
+        <v>1994.157741</v>
+      </c>
+      <c r="F18">
+        <f>XMP_GET!B13</f>
+        <v>1168.782993</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7">
       <c r="A19">
         <v>16384</v>
       </c>
@@ -1501,15 +1987,23 @@
         <v>1185.5282199999999</v>
       </c>
       <c r="C19">
-        <f>K_PUT!B14</f>
-        <v>2878.678731</v>
+        <f>FUJITSU_PUT!B14</f>
+        <v>2965.1615240000001</v>
       </c>
       <c r="D19">
-        <f>K_GET!B14</f>
+        <f>FUJITSU_GET!B14</f>
         <v>1855.17749</v>
       </c>
-    </row>
-    <row r="20" spans="1:4">
+      <c r="E19">
+        <f>XMP_PUT!B14</f>
+        <v>2795.9044370000001</v>
+      </c>
+      <c r="F19">
+        <f>XMP_GET!B14</f>
+        <v>1876.961851</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7">
       <c r="A20">
         <v>32768</v>
       </c>
@@ -1518,15 +2012,23 @@
         <v>1885.385501</v>
       </c>
       <c r="C20">
-        <f>K_PUT!B15</f>
-        <v>3589.8334789999999</v>
+        <f>FUJITSU_PUT!B15</f>
+        <v>3652.4549959999999</v>
       </c>
       <c r="D20">
-        <f>K_GET!B15</f>
+        <f>FUJITSU_GET!B15</f>
         <v>2670.2522100000001</v>
       </c>
-    </row>
-    <row r="21" spans="1:4">
+      <c r="E20">
+        <f>XMP_PUT!B15</f>
+        <v>3492.0871740000002</v>
+      </c>
+      <c r="F20">
+        <f>XMP_GET!B15</f>
+        <v>2690.7538180000001</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7">
       <c r="A21">
         <v>65536</v>
       </c>
@@ -1535,15 +2037,23 @@
         <v>2705.0252810000002</v>
       </c>
       <c r="C21">
-        <f>K_PUT!B16</f>
-        <v>4093.0581139999999</v>
+        <f>FUJITSU_PUT!B16</f>
+        <v>4133.9809500000001</v>
       </c>
       <c r="D21">
-        <f>K_GET!B16</f>
+        <f>FUJITSU_GET!B16</f>
         <v>3422.1560789999999</v>
       </c>
-    </row>
-    <row r="22" spans="1:4">
+      <c r="E21">
+        <f>XMP_PUT!B16</f>
+        <v>3997.9258810000001</v>
+      </c>
+      <c r="F21">
+        <f>XMP_GET!B16</f>
+        <v>3437.9540980000002</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7">
       <c r="A22">
         <v>131072</v>
       </c>
@@ -1552,15 +2062,23 @@
         <v>3455.2188639999999</v>
       </c>
       <c r="C22">
-        <f>K_PUT!B17</f>
-        <v>4402.5258629999998</v>
+        <f>FUJITSU_PUT!B17</f>
+        <v>4426.1641849999996</v>
       </c>
       <c r="D22">
-        <f>K_GET!B17</f>
+        <f>FUJITSU_GET!B17</f>
         <v>3981.0472599999998</v>
       </c>
-    </row>
-    <row r="23" spans="1:4">
+      <c r="E22">
+        <f>XMP_PUT!B17</f>
+        <v>4314.275369</v>
+      </c>
+      <c r="F22">
+        <f>XMP_GET!B17</f>
+        <v>3993.4798839999999</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7">
       <c r="A23">
         <v>262144</v>
       </c>
@@ -1569,15 +2087,23 @@
         <v>4010.6177089999996</v>
       </c>
       <c r="C23">
-        <f>K_PUT!B18</f>
-        <v>4575.0187610000003</v>
+        <f>FUJITSU_PUT!B18</f>
+        <v>4587.8698249999998</v>
       </c>
       <c r="D23">
-        <f>K_GET!B18</f>
+        <f>FUJITSU_GET!B18</f>
         <v>4336.8295669999998</v>
       </c>
-    </row>
-    <row r="24" spans="1:4">
+      <c r="E23">
+        <f>XMP_PUT!B18</f>
+        <v>4492.2286009999998</v>
+      </c>
+      <c r="F23">
+        <f>XMP_GET!B18</f>
+        <v>4343.4763519999997</v>
+      </c>
+    </row>
+    <row r="24" spans="1:7">
       <c r="A24">
         <v>524288</v>
       </c>
@@ -1586,15 +2112,23 @@
         <v>4346.5911679999999</v>
       </c>
       <c r="C24">
-        <f>K_PUT!B19</f>
-        <v>4666.019953</v>
+        <f>FUJITSU_PUT!B19</f>
+        <v>4673.1526009999998</v>
       </c>
       <c r="D24">
-        <f>K_GET!B19</f>
+        <f>FUJITSU_GET!B19</f>
         <v>4537.1687699999993</v>
       </c>
-    </row>
-    <row r="25" spans="1:4">
+      <c r="E24">
+        <f>XMP_PUT!B19</f>
+        <v>4586.6657340000002</v>
+      </c>
+      <c r="F24">
+        <f>XMP_GET!B19</f>
+        <v>4541.2166200000001</v>
+      </c>
+    </row>
+    <row r="25" spans="1:7">
       <c r="A25">
         <v>1048576</v>
       </c>
@@ -1603,15 +2137,23 @@
         <v>4543.3908959999999</v>
       </c>
       <c r="C25">
-        <f>K_PUT!B20</f>
-        <v>4713.7815860000001</v>
+        <f>FUJITSU_PUT!B20</f>
+        <v>4716.919852</v>
       </c>
       <c r="D25">
-        <f>K_GET!B20</f>
+        <f>FUJITSU_GET!B20</f>
         <v>4646.8927679999997</v>
       </c>
-    </row>
-    <row r="26" spans="1:4">
+      <c r="E25">
+        <f>XMP_PUT!B20</f>
+        <v>4636.2806330000003</v>
+      </c>
+      <c r="F25">
+        <f>XMP_GET!B20</f>
+        <v>4649.2518949999994</v>
+      </c>
+    </row>
+    <row r="26" spans="1:7">
       <c r="A26">
         <v>2097152</v>
       </c>
@@ -1620,15 +2162,23 @@
         <v>4648.8499529999999</v>
       </c>
       <c r="C26">
-        <f>K_PUT!B21</f>
-        <v>4737.7847659999998</v>
+        <f>FUJITSU_PUT!B21</f>
+        <v>4739.3586849999992</v>
       </c>
       <c r="D26">
-        <f>K_GET!B21</f>
+        <f>FUJITSU_GET!B21</f>
         <v>4702.9306530000003</v>
       </c>
-    </row>
-    <row r="27" spans="1:4">
+      <c r="E26">
+        <f>XMP_PUT!B21</f>
+        <v>4661.6844869999995</v>
+      </c>
+      <c r="F26">
+        <f>XMP_GET!B21</f>
+        <v>4704.1912940000002</v>
+      </c>
+    </row>
+    <row r="27" spans="1:7">
       <c r="A27">
         <v>4194304</v>
       </c>
@@ -1637,15 +2187,23 @@
         <v>4705.6004249999996</v>
       </c>
       <c r="C27">
-        <f>K_PUT!B22</f>
-        <v>4749.8459869999997</v>
+        <f>FUJITSU_PUT!B22</f>
+        <v>4750.5480459999999</v>
       </c>
       <c r="D27">
-        <f>K_GET!B22</f>
+        <f>FUJITSU_GET!B22</f>
         <v>4732.4150890000001</v>
       </c>
-    </row>
-    <row r="28" spans="1:4">
+      <c r="E27">
+        <f>XMP_PUT!B22</f>
+        <v>4674.5093320000005</v>
+      </c>
+      <c r="F27">
+        <f>XMP_GET!B22</f>
+        <v>4732.852973</v>
+      </c>
+    </row>
+    <row r="28" spans="1:7">
       <c r="A28">
         <v>8388608</v>
       </c>
@@ -1654,12 +2212,25 @@
         <v>4733.3229890000002</v>
       </c>
       <c r="C28">
-        <f>K_PUT!B23</f>
-        <v>4755.9522340000003</v>
+        <f>FUJITSU_PUT!B23</f>
+        <v>4756.1652599999998</v>
       </c>
       <c r="D28">
-        <f>K_GET!B23</f>
+        <f>FUJITSU_GET!B23</f>
         <v>4746.5711080000001</v>
+      </c>
+      <c r="E28">
+        <f>XMP_PUT!B23</f>
+        <v>4680.9560889999993</v>
+      </c>
+      <c r="F28">
+        <f>XMP_GET!B23</f>
+        <v>4746.8544749999992</v>
+      </c>
+    </row>
+    <row r="29" spans="1:7">
+      <c r="G29" t="s">
+        <v>11</v>
       </c>
     </row>
   </sheetData>
@@ -2676,7 +3247,7 @@
   <dimension ref="A1:L23"/>
   <sheetViews>
     <sheetView showRuler="0" workbookViewId="0">
-      <selection activeCell="A23" sqref="A23"/>
+      <selection activeCell="L2" sqref="L2:L23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="12" defaultRowHeight="18" x14ac:dyDescent="0"/>
@@ -2725,37 +3296,37 @@
       </c>
       <c r="B2">
         <f t="shared" ref="B2:B23" si="0">MAX(C2:L2)/1000/1000</f>
-        <v>3.5987399999999998</v>
+        <v>3.664682</v>
       </c>
       <c r="C2">
-        <v>3561888</v>
+        <v>3636364</v>
       </c>
       <c r="D2">
-        <v>3571429</v>
+        <v>3624830</v>
       </c>
       <c r="E2">
-        <v>3568243</v>
+        <v>3626473</v>
       </c>
       <c r="F2">
-        <v>3565062</v>
+        <v>3657979</v>
       </c>
       <c r="G2">
-        <v>3598740</v>
+        <v>3654637</v>
       </c>
       <c r="H2">
-        <v>3565062</v>
+        <v>3613369</v>
       </c>
       <c r="I2">
-        <v>3568243</v>
+        <v>3633061</v>
       </c>
       <c r="J2">
-        <v>3568243</v>
+        <v>3661327</v>
       </c>
       <c r="K2">
-        <v>3584229</v>
+        <v>3664682</v>
       </c>
       <c r="L2">
-        <v>3573024</v>
+        <v>3642987</v>
       </c>
     </row>
     <row r="3" spans="1:12">
@@ -2764,37 +3335,37 @@
       </c>
       <c r="B3">
         <f t="shared" si="0"/>
-        <v>7.3026020000000003</v>
+        <v>7.4487899999999998</v>
       </c>
       <c r="C3">
-        <v>7259528</v>
+        <v>7448790</v>
       </c>
       <c r="D3">
-        <v>7302602</v>
+        <v>7434944</v>
       </c>
       <c r="E3">
-        <v>7299270</v>
+        <v>7438401</v>
       </c>
       <c r="F3">
-        <v>7262823</v>
+        <v>7434944</v>
       </c>
       <c r="G3">
-        <v>7276035</v>
+        <v>7438401</v>
       </c>
       <c r="H3">
-        <v>7289294</v>
+        <v>7441860</v>
       </c>
       <c r="I3">
-        <v>7272727</v>
+        <v>6849315</v>
       </c>
       <c r="J3">
-        <v>7299270</v>
+        <v>7431491</v>
       </c>
       <c r="K3">
-        <v>7299270</v>
+        <v>7428041</v>
       </c>
       <c r="L3">
-        <v>7269423</v>
+        <v>6855184</v>
       </c>
     </row>
     <row r="4" spans="1:12">
@@ -2803,37 +3374,37 @@
       </c>
       <c r="B4">
         <f t="shared" si="0"/>
-        <v>14.103129000000001</v>
+        <v>14.375562</v>
       </c>
       <c r="C4">
-        <v>14072120</v>
+        <v>14247551</v>
       </c>
       <c r="D4">
-        <v>14084507</v>
+        <v>14234875</v>
       </c>
       <c r="E4">
-        <v>14010508</v>
+        <v>14272971</v>
       </c>
       <c r="F4">
-        <v>14103129</v>
+        <v>14260250</v>
       </c>
       <c r="G4">
-        <v>13986014</v>
+        <v>14304873</v>
       </c>
       <c r="H4">
-        <v>14084507</v>
+        <v>14317673</v>
       </c>
       <c r="I4">
-        <v>14059754</v>
+        <v>14279340</v>
       </c>
       <c r="J4">
-        <v>14059754</v>
+        <v>14115571</v>
       </c>
       <c r="K4">
-        <v>14078311</v>
+        <v>14298481</v>
       </c>
       <c r="L4">
-        <v>14041246</v>
+        <v>14375562</v>
       </c>
     </row>
     <row r="5" spans="1:12">
@@ -2842,37 +3413,37 @@
       </c>
       <c r="B5">
         <f t="shared" si="0"/>
-        <v>28.393965999999999</v>
+        <v>28.764044999999999</v>
       </c>
       <c r="C5">
-        <v>28156621</v>
+        <v>28520499</v>
       </c>
       <c r="D5">
-        <v>27911034</v>
+        <v>28584189</v>
       </c>
       <c r="E5">
-        <v>28181418</v>
+        <v>28533214</v>
       </c>
       <c r="F5">
-        <v>28206258</v>
+        <v>28635347</v>
       </c>
       <c r="G5">
-        <v>28193833</v>
+        <v>28545941</v>
       </c>
       <c r="H5">
-        <v>28169014</v>
+        <v>28507795</v>
       </c>
       <c r="I5">
-        <v>28193833</v>
+        <v>28495102</v>
       </c>
       <c r="J5">
-        <v>28206258</v>
+        <v>28596962</v>
       </c>
       <c r="K5">
-        <v>28393966</v>
+        <v>28764045</v>
       </c>
       <c r="L5">
-        <v>28169014</v>
+        <v>28699552</v>
       </c>
     </row>
     <row r="6" spans="1:12">
@@ -2881,37 +3452,37 @@
       </c>
       <c r="B6">
         <f t="shared" si="0"/>
-        <v>43.671101999999998</v>
+        <v>44.107512</v>
       </c>
       <c r="C6">
-        <v>43493034</v>
+        <v>44016506</v>
       </c>
       <c r="D6">
-        <v>43567052</v>
+        <v>43956044</v>
       </c>
       <c r="E6">
-        <v>43567052</v>
+        <v>43956044</v>
       </c>
       <c r="F6">
-        <v>43581886</v>
+        <v>43971144</v>
       </c>
       <c r="G6">
-        <v>43611584</v>
+        <v>44061962</v>
       </c>
       <c r="H6">
-        <v>43596730</v>
+        <v>43880699</v>
       </c>
       <c r="I6">
-        <v>43537415</v>
+        <v>43895748</v>
       </c>
       <c r="J6">
-        <v>43611584</v>
+        <v>43895748</v>
       </c>
       <c r="K6">
-        <v>43671102</v>
+        <v>44107512</v>
       </c>
       <c r="L6">
-        <v>43493034</v>
+        <v>43745728</v>
       </c>
     </row>
     <row r="7" spans="1:12">
@@ -2920,37 +3491,37 @@
       </c>
       <c r="B7">
         <f t="shared" si="0"/>
-        <v>79.975008000000003</v>
+        <v>96.859628999999998</v>
       </c>
       <c r="C7">
-        <v>79925070</v>
+        <v>96204434</v>
       </c>
       <c r="D7">
-        <v>79800499</v>
+        <v>95988001</v>
       </c>
       <c r="E7">
-        <v>78987967</v>
+        <v>96421846</v>
       </c>
       <c r="F7">
-        <v>79925070</v>
+        <v>96240602</v>
       </c>
       <c r="G7">
-        <v>78987967</v>
+        <v>95380030</v>
       </c>
       <c r="H7">
-        <v>79975008</v>
+        <v>96530920</v>
       </c>
       <c r="I7">
-        <v>79950031</v>
+        <v>96385542</v>
       </c>
       <c r="J7">
-        <v>79183421</v>
+        <v>95736724</v>
       </c>
       <c r="K7">
-        <v>79850281</v>
+        <v>96640242</v>
       </c>
       <c r="L7">
-        <v>78914920</v>
+        <v>96859629</v>
       </c>
     </row>
     <row r="8" spans="1:12">
@@ -2959,37 +3530,37 @@
       </c>
       <c r="B8">
         <f t="shared" si="0"/>
-        <v>153.84615400000001</v>
+        <v>172.04301100000001</v>
       </c>
       <c r="C8">
-        <v>153569286</v>
+        <v>169705005</v>
       </c>
       <c r="D8">
-        <v>153615362</v>
+        <v>169873922</v>
       </c>
       <c r="E8">
-        <v>153661465</v>
+        <v>171122995</v>
       </c>
       <c r="F8">
-        <v>153846154</v>
+        <v>171466845</v>
       </c>
       <c r="G8">
-        <v>153846154</v>
+        <v>171409441</v>
       </c>
       <c r="H8">
-        <v>152199762</v>
+        <v>171352075</v>
       </c>
       <c r="I8">
-        <v>152608048</v>
+        <v>171180207</v>
       </c>
       <c r="J8">
-        <v>153661465</v>
+        <v>171524288</v>
       </c>
       <c r="K8">
-        <v>153247531</v>
+        <v>170099668</v>
       </c>
       <c r="L8">
-        <v>153661465</v>
+        <v>172043011</v>
       </c>
     </row>
     <row r="9" spans="1:12">
@@ -2998,37 +3569,37 @@
       </c>
       <c r="B9">
         <f t="shared" si="0"/>
-        <v>284.68167900000003</v>
+        <v>317.51938000000001</v>
       </c>
       <c r="C9">
-        <v>283185841</v>
+        <v>317224287</v>
       </c>
       <c r="D9">
-        <v>283971159</v>
+        <v>317519380</v>
       </c>
       <c r="E9">
-        <v>283656510</v>
+        <v>317224287</v>
       </c>
       <c r="F9">
-        <v>280240832</v>
+        <v>317322591</v>
       </c>
       <c r="G9">
-        <v>283420980</v>
+        <v>316342292</v>
       </c>
       <c r="H9">
-        <v>283735107</v>
+        <v>317322591</v>
       </c>
       <c r="I9">
-        <v>283735107</v>
+        <v>317126045</v>
       </c>
       <c r="J9">
-        <v>280547945</v>
+        <v>316635745</v>
       </c>
       <c r="K9">
-        <v>284681679</v>
+        <v>317519380</v>
       </c>
       <c r="L9">
-        <v>280778722</v>
+        <v>316831683</v>
       </c>
     </row>
     <row r="10" spans="1:12">
@@ -3037,37 +3608,37 @@
       </c>
       <c r="B10">
         <f t="shared" si="0"/>
-        <v>483.81762300000003</v>
+        <v>521.91641200000004</v>
       </c>
       <c r="C10">
-        <v>483703354</v>
+        <v>520193040</v>
       </c>
       <c r="D10">
-        <v>483360869</v>
+        <v>518743668</v>
       </c>
       <c r="E10">
-        <v>483817623</v>
+        <v>521384929</v>
       </c>
       <c r="F10">
-        <v>483817623</v>
+        <v>521916412</v>
       </c>
       <c r="G10">
-        <v>483817623</v>
+        <v>520854527</v>
       </c>
       <c r="H10">
-        <v>477834811</v>
+        <v>521252227</v>
       </c>
       <c r="I10">
-        <v>481203008</v>
+        <v>520854527</v>
       </c>
       <c r="J10">
-        <v>483246815</v>
+        <v>521650535</v>
       </c>
       <c r="K10">
-        <v>479064327</v>
+        <v>514185287</v>
       </c>
       <c r="L10">
-        <v>483817623</v>
+        <v>521916412</v>
       </c>
     </row>
     <row r="11" spans="1:12">
@@ -3076,37 +3647,37 @@
       </c>
       <c r="B11">
         <f t="shared" si="0"/>
-        <v>764.46435199999996</v>
+        <v>814.31411500000002</v>
       </c>
       <c r="C11">
-        <v>763324637</v>
+        <v>813021040</v>
       </c>
       <c r="D11">
-        <v>762046512</v>
+        <v>813343924</v>
       </c>
       <c r="E11">
-        <v>762330169</v>
+        <v>813182450</v>
       </c>
       <c r="F11">
-        <v>763894069</v>
+        <v>812537195</v>
       </c>
       <c r="G11">
-        <v>763040238</v>
+        <v>812214951</v>
       </c>
       <c r="H11">
-        <v>764464352</v>
+        <v>812376041</v>
       </c>
       <c r="I11">
-        <v>764036560</v>
+        <v>812859694</v>
       </c>
       <c r="J11">
-        <v>763182411</v>
+        <v>812053925</v>
       </c>
       <c r="K11">
-        <v>762614038</v>
+        <v>814314115</v>
       </c>
       <c r="L11">
-        <v>763466915</v>
+        <v>810607560</v>
       </c>
     </row>
     <row r="12" spans="1:12">
@@ -3115,37 +3686,37 @@
       </c>
       <c r="B12">
         <f t="shared" si="0"/>
-        <v>1309.2536359999999</v>
+        <v>1392.013594</v>
       </c>
       <c r="C12">
-        <v>1306955967</v>
+        <v>1391540683</v>
       </c>
       <c r="D12">
-        <v>1308208240</v>
+        <v>1391540683</v>
       </c>
       <c r="E12">
-        <v>1307790549</v>
+        <v>1390595824</v>
       </c>
       <c r="F12">
-        <v>1305914236</v>
+        <v>1392013594</v>
       </c>
       <c r="G12">
-        <v>1308835277</v>
+        <v>1391777098</v>
       </c>
       <c r="H12">
-        <v>1307373125</v>
+        <v>1391068093</v>
       </c>
       <c r="I12">
-        <v>1307790549</v>
+        <v>1390123876</v>
       </c>
       <c r="J12">
-        <v>1305082046</v>
+        <v>1392013594</v>
       </c>
       <c r="K12">
-        <v>1309253636</v>
+        <v>1389416554</v>
       </c>
       <c r="L12">
-        <v>1307581804</v>
+        <v>1390123876</v>
       </c>
     </row>
     <row r="13" spans="1:12">
@@ -3154,37 +3725,37 @@
       </c>
       <c r="B13">
         <f t="shared" si="0"/>
-        <v>2063.9959690000001</v>
+        <v>2151.2605040000003</v>
       </c>
       <c r="C13">
-        <v>2060880503</v>
+        <v>2149285058</v>
       </c>
       <c r="D13">
-        <v>2062437059</v>
+        <v>2149003148</v>
       </c>
       <c r="E13">
-        <v>2061658487</v>
+        <v>2148721311</v>
       </c>
       <c r="F13">
-        <v>2061917946</v>
+        <v>2149567043</v>
       </c>
       <c r="G13">
-        <v>2062177470</v>
+        <v>2149285058</v>
       </c>
       <c r="H13">
-        <v>2061399094</v>
+        <v>2147594704</v>
       </c>
       <c r="I13">
-        <v>2059585167</v>
+        <v>2148157860</v>
       </c>
       <c r="J13">
-        <v>2060103106</v>
+        <v>2148157860</v>
       </c>
       <c r="K13">
-        <v>2063995969</v>
+        <v>2149567043</v>
       </c>
       <c r="L13">
-        <v>2060621305</v>
+        <v>2151260504</v>
       </c>
     </row>
     <row r="14" spans="1:12">
@@ -3193,37 +3764,37 @@
       </c>
       <c r="B14">
         <f t="shared" si="0"/>
-        <v>2878.678731</v>
+        <v>2965.1615240000001</v>
       </c>
       <c r="C14">
-        <v>2877667516</v>
+        <v>2959804896</v>
       </c>
       <c r="D14">
-        <v>2877414823</v>
+        <v>2959003070</v>
       </c>
       <c r="E14">
-        <v>2876657010</v>
+        <v>2958468761</v>
       </c>
       <c r="F14">
-        <v>2877920253</v>
+        <v>2964088648</v>
       </c>
       <c r="G14">
-        <v>2878173035</v>
+        <v>2960072267</v>
       </c>
       <c r="H14">
-        <v>2876404494</v>
+        <v>2959537572</v>
       </c>
       <c r="I14">
-        <v>2874133848</v>
+        <v>2965161524</v>
       </c>
       <c r="J14">
-        <v>2873125822</v>
+        <v>2960874672</v>
       </c>
       <c r="K14">
-        <v>2878678731</v>
+        <v>2965161524</v>
       </c>
       <c r="L14">
-        <v>2878173035</v>
+        <v>2964356794</v>
       </c>
     </row>
     <row r="15" spans="1:12">
@@ -3232,37 +3803,37 @@
       </c>
       <c r="B15">
         <f t="shared" si="0"/>
-        <v>3589.8334789999999</v>
+        <v>3652.4549959999999</v>
       </c>
       <c r="C15">
-        <v>3584336032</v>
+        <v>3652047924</v>
       </c>
       <c r="D15">
-        <v>3586690018</v>
+        <v>3652251449</v>
       </c>
       <c r="E15">
-        <v>3583356116</v>
+        <v>3651030641</v>
       </c>
       <c r="F15">
-        <v>3586101231</v>
+        <v>3651030641</v>
       </c>
       <c r="G15">
-        <v>3584924238</v>
+        <v>3649200958</v>
       </c>
       <c r="H15">
-        <v>3588064604</v>
+        <v>3650420543</v>
       </c>
       <c r="I15">
-        <v>3586493734</v>
+        <v>3649810648</v>
       </c>
       <c r="J15">
-        <v>3587082649</v>
+        <v>3651640943</v>
       </c>
       <c r="K15">
-        <v>3589833479</v>
+        <v>3647982188</v>
       </c>
       <c r="L15">
-        <v>3587082649</v>
+        <v>3652454996</v>
       </c>
     </row>
     <row r="16" spans="1:12">
@@ -3271,37 +3842,37 @@
       </c>
       <c r="B16">
         <f t="shared" si="0"/>
-        <v>4093.0581139999999</v>
+        <v>4133.9809500000001</v>
       </c>
       <c r="C16">
-        <v>4091524895</v>
+        <v>4133198789</v>
       </c>
       <c r="D16">
-        <v>4090886392</v>
+        <v>4133329129</v>
       </c>
       <c r="E16">
-        <v>4091780352</v>
+        <v>4133850569</v>
       </c>
       <c r="F16">
-        <v>4091780352</v>
+        <v>4132416924</v>
       </c>
       <c r="G16">
-        <v>4091908092</v>
+        <v>4133459477</v>
       </c>
       <c r="H16">
-        <v>4091652619</v>
+        <v>4132286642</v>
       </c>
       <c r="I16">
-        <v>4091524895</v>
+        <v>4133459477</v>
       </c>
       <c r="J16">
-        <v>4091014077</v>
+        <v>4133459477</v>
       </c>
       <c r="K16">
-        <v>4093058114</v>
+        <v>4133980950</v>
       </c>
       <c r="L16">
-        <v>4091908092</v>
+        <v>4133980950</v>
       </c>
     </row>
     <row r="17" spans="1:12">
@@ -3310,37 +3881,37 @@
       </c>
       <c r="B17">
         <f t="shared" si="0"/>
-        <v>4402.5258629999998</v>
+        <v>4426.1641849999996</v>
       </c>
       <c r="C17">
-        <v>4401417082</v>
+        <v>4425939996</v>
       </c>
       <c r="D17">
-        <v>4401786614</v>
+        <v>4426014723</v>
       </c>
       <c r="E17">
-        <v>4401860528</v>
+        <v>4425939996</v>
       </c>
       <c r="F17">
-        <v>4401860528</v>
+        <v>4426014723</v>
       </c>
       <c r="G17">
-        <v>4402082284</v>
+        <v>4425267565</v>
       </c>
       <c r="H17">
-        <v>4401564887</v>
+        <v>4425939996</v>
       </c>
       <c r="I17">
-        <v>4401860528</v>
+        <v>4425865271</v>
       </c>
       <c r="J17">
-        <v>4402008363</v>
+        <v>4425790549</v>
       </c>
       <c r="K17">
-        <v>4402525863</v>
+        <v>4425939996</v>
       </c>
       <c r="L17">
-        <v>4402156207</v>
+        <v>4426164185</v>
       </c>
     </row>
     <row r="18" spans="1:12">
@@ -3349,37 +3920,37 @@
       </c>
       <c r="B18">
         <f t="shared" si="0"/>
-        <v>4575.0187610000003</v>
+        <v>4587.8698249999998</v>
       </c>
       <c r="C18">
-        <v>4574779240</v>
+        <v>4587709243</v>
       </c>
       <c r="D18">
-        <v>4574739322</v>
+        <v>4587789533</v>
       </c>
       <c r="E18">
-        <v>4574699405</v>
+        <v>4587709243</v>
       </c>
       <c r="F18">
-        <v>4574779240</v>
+        <v>4587789533</v>
       </c>
       <c r="G18">
-        <v>4574779240</v>
+        <v>4587709243</v>
       </c>
       <c r="H18">
-        <v>4574699405</v>
+        <v>4587709243</v>
       </c>
       <c r="I18">
-        <v>4574739322</v>
+        <v>4587669099</v>
       </c>
       <c r="J18">
-        <v>4574539743</v>
+        <v>4587347974</v>
       </c>
       <c r="K18">
-        <v>4575018761</v>
+        <v>4587869825</v>
       </c>
       <c r="L18">
-        <v>4574938918</v>
+        <v>4587829679</v>
       </c>
     </row>
     <row r="19" spans="1:12">
@@ -3388,37 +3959,37 @@
       </c>
       <c r="B19">
         <f t="shared" si="0"/>
-        <v>4666.019953</v>
+        <v>4673.1526009999998</v>
       </c>
       <c r="C19">
-        <v>4665791570</v>
+        <v>4673090121</v>
       </c>
       <c r="D19">
-        <v>4665853854</v>
+        <v>4673069295</v>
       </c>
       <c r="E19">
-        <v>4665770809</v>
+        <v>4673048470</v>
       </c>
       <c r="F19">
-        <v>4665853854</v>
+        <v>4673069295</v>
       </c>
       <c r="G19">
-        <v>4665936902</v>
+        <v>4673110948</v>
       </c>
       <c r="H19">
-        <v>4665812331</v>
+        <v>4673090121</v>
       </c>
       <c r="I19">
-        <v>4665729287</v>
+        <v>4673069295</v>
       </c>
       <c r="J19">
-        <v>4665750048</v>
+        <v>4673069295</v>
       </c>
       <c r="K19">
-        <v>4665687766</v>
+        <v>4673152601</v>
       </c>
       <c r="L19">
-        <v>4666019953</v>
+        <v>4673110948</v>
       </c>
     </row>
     <row r="20" spans="1:12">
@@ -3427,37 +3998,37 @@
       </c>
       <c r="B20">
         <f t="shared" si="0"/>
-        <v>4713.7815860000001</v>
+        <v>4716.919852</v>
       </c>
       <c r="C20">
-        <v>4712997672</v>
+        <v>4716898633</v>
       </c>
       <c r="D20">
-        <v>4711218942</v>
+        <v>4716919852</v>
       </c>
       <c r="E20">
-        <v>4713760396</v>
+        <v>4716834979</v>
       </c>
       <c r="F20">
-        <v>4712203430</v>
+        <v>4716909243</v>
       </c>
       <c r="G20">
-        <v>4713739205</v>
+        <v>4716898633</v>
       </c>
       <c r="H20">
-        <v>4713431970</v>
+        <v>4716845588</v>
       </c>
       <c r="I20">
-        <v>4711832876</v>
+        <v>4716877415</v>
       </c>
       <c r="J20">
-        <v>4712574043</v>
+        <v>4716898633</v>
       </c>
       <c r="K20">
-        <v>4713781586</v>
+        <v>4716898633</v>
       </c>
       <c r="L20">
-        <v>4713135368</v>
+        <v>4716909243</v>
       </c>
     </row>
     <row r="21" spans="1:12">
@@ -3466,37 +4037,37 @@
       </c>
       <c r="B21">
         <f t="shared" si="0"/>
-        <v>4737.7847659999998</v>
+        <v>4739.3586849999992</v>
       </c>
       <c r="C21">
-        <v>4737661680</v>
+        <v>4739326554</v>
       </c>
       <c r="D21">
-        <v>4737645626</v>
+        <v>4739358685</v>
       </c>
       <c r="E21">
-        <v>4737640275</v>
+        <v>4739331909</v>
       </c>
       <c r="F21">
-        <v>4737645626</v>
+        <v>4739326554</v>
       </c>
       <c r="G21">
-        <v>4737624221</v>
+        <v>4739342619</v>
       </c>
       <c r="H21">
-        <v>4737533250</v>
+        <v>4739326554</v>
       </c>
       <c r="I21">
-        <v>4737538601</v>
+        <v>4739342619</v>
       </c>
       <c r="J21">
-        <v>4737511846</v>
+        <v>4739347974</v>
       </c>
       <c r="K21">
-        <v>4737543952</v>
+        <v>4739353330</v>
       </c>
       <c r="L21">
-        <v>4737784766</v>
+        <v>4739326554</v>
       </c>
     </row>
     <row r="22" spans="1:12">
@@ -3505,37 +4076,37 @@
       </c>
       <c r="B22">
         <f t="shared" si="0"/>
-        <v>4749.8459869999997</v>
+        <v>4750.5480459999999</v>
       </c>
       <c r="C22">
-        <v>4749714205</v>
+        <v>4750529214</v>
       </c>
       <c r="D22">
-        <v>4749711516</v>
+        <v>4750537285</v>
       </c>
       <c r="E22">
-        <v>4749695380</v>
+        <v>4750545356</v>
       </c>
       <c r="F22">
-        <v>4749660419</v>
+        <v>4750537285</v>
       </c>
       <c r="G22">
-        <v>4749644284</v>
+        <v>4750548046</v>
       </c>
       <c r="H22">
-        <v>4749614702</v>
+        <v>4750542665</v>
       </c>
       <c r="I22">
-        <v>4749598567</v>
+        <v>4750548046</v>
       </c>
       <c r="J22">
-        <v>4749574364</v>
+        <v>4750531904</v>
       </c>
       <c r="K22">
-        <v>4749571675</v>
+        <v>4750537285</v>
       </c>
       <c r="L22">
-        <v>4749845987</v>
+        <v>4750539975</v>
       </c>
     </row>
     <row r="23" spans="1:12">
@@ -3544,37 +4115,37 @@
       </c>
       <c r="B23">
         <f t="shared" si="0"/>
-        <v>4755.9522340000003</v>
+        <v>4756.1652599999998</v>
       </c>
       <c r="C23">
-        <v>4755832247</v>
+        <v>4756149080</v>
       </c>
       <c r="D23">
-        <v>4755824158</v>
+        <v>4756155821</v>
       </c>
       <c r="E23">
-        <v>4755810677</v>
+        <v>4756165260</v>
       </c>
       <c r="F23">
-        <v>4755795848</v>
+        <v>4756157170</v>
       </c>
       <c r="G23">
-        <v>4755789107</v>
+        <v>4756161215</v>
       </c>
       <c r="H23">
-        <v>4755720355</v>
+        <v>4756158518</v>
       </c>
       <c r="I23">
-        <v>4755708222</v>
+        <v>4756159866</v>
       </c>
       <c r="J23">
-        <v>4755692045</v>
+        <v>4756145035</v>
       </c>
       <c r="K23">
-        <v>4755683957</v>
+        <v>4756155821</v>
       </c>
       <c r="L23">
-        <v>4755952234</v>
+        <v>4756157170</v>
       </c>
     </row>
   </sheetData>
@@ -4505,4 +5076,1840 @@
     </ext>
   </extLst>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:L23"/>
+  <sheetViews>
+    <sheetView showRuler="0" workbookViewId="0">
+      <selection activeCell="B2" sqref="B2:B23"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="12" defaultRowHeight="18" x14ac:dyDescent="0"/>
+  <sheetData>
+    <row r="1" spans="1:12">
+      <c r="A1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1">
+        <v>1</v>
+      </c>
+      <c r="D1">
+        <v>2</v>
+      </c>
+      <c r="E1">
+        <v>3</v>
+      </c>
+      <c r="F1">
+        <v>4</v>
+      </c>
+      <c r="G1">
+        <v>5</v>
+      </c>
+      <c r="H1">
+        <v>6</v>
+      </c>
+      <c r="I1">
+        <v>7</v>
+      </c>
+      <c r="J1">
+        <v>8</v>
+      </c>
+      <c r="K1">
+        <v>9</v>
+      </c>
+      <c r="L1">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="2" spans="1:12">
+      <c r="A2">
+        <v>4</v>
+      </c>
+      <c r="B2">
+        <f t="shared" ref="B2:B23" si="0">MAX(C2:L2)/1000/1000</f>
+        <v>3.5366930000000001</v>
+      </c>
+      <c r="C2">
+        <v>3524229</v>
+      </c>
+      <c r="D2">
+        <v>3525782</v>
+      </c>
+      <c r="E2">
+        <v>3498032</v>
+      </c>
+      <c r="F2">
+        <v>3518030</v>
+      </c>
+      <c r="G2">
+        <v>3507234</v>
+      </c>
+      <c r="H2">
+        <v>3536693</v>
+      </c>
+      <c r="I2">
+        <v>3513395</v>
+      </c>
+      <c r="J2">
+        <v>3473730</v>
+      </c>
+      <c r="K2">
+        <v>3522677</v>
+      </c>
+      <c r="L2">
+        <v>3472222</v>
+      </c>
+    </row>
+    <row r="3" spans="1:12">
+      <c r="A3">
+        <v>8</v>
+      </c>
+      <c r="B3">
+        <f t="shared" si="0"/>
+        <v>7.1652490000000002</v>
+      </c>
+      <c r="C3">
+        <v>7162041</v>
+      </c>
+      <c r="D3">
+        <v>7155635</v>
+      </c>
+      <c r="E3">
+        <v>6625259</v>
+      </c>
+      <c r="F3">
+        <v>6600660</v>
+      </c>
+      <c r="G3">
+        <v>7060900</v>
+      </c>
+      <c r="H3">
+        <v>7130125</v>
+      </c>
+      <c r="I3">
+        <v>7057786</v>
+      </c>
+      <c r="J3">
+        <v>7165249</v>
+      </c>
+      <c r="K3">
+        <v>7162041</v>
+      </c>
+      <c r="L3">
+        <v>6606111</v>
+      </c>
+    </row>
+    <row r="4" spans="1:12">
+      <c r="A4">
+        <v>16</v>
+      </c>
+      <c r="B4">
+        <f t="shared" si="0"/>
+        <v>13.769363</v>
+      </c>
+      <c r="C4">
+        <v>13745704</v>
+      </c>
+      <c r="D4">
+        <v>13559322</v>
+      </c>
+      <c r="E4">
+        <v>13769363</v>
+      </c>
+      <c r="F4">
+        <v>13599660</v>
+      </c>
+      <c r="G4">
+        <v>13733906</v>
+      </c>
+      <c r="H4">
+        <v>13565070</v>
+      </c>
+      <c r="I4">
+        <v>13757524</v>
+      </c>
+      <c r="J4">
+        <v>13692769</v>
+      </c>
+      <c r="K4">
+        <v>13745704</v>
+      </c>
+      <c r="L4">
+        <v>13739802</v>
+      </c>
+    </row>
+    <row r="5" spans="1:12">
+      <c r="A5">
+        <v>32</v>
+      </c>
+      <c r="B5">
+        <f t="shared" si="0"/>
+        <v>27.280476999999998</v>
+      </c>
+      <c r="C5">
+        <v>27210884</v>
+      </c>
+      <c r="D5">
+        <v>27245636</v>
+      </c>
+      <c r="E5">
+        <v>27187766</v>
+      </c>
+      <c r="F5">
+        <v>27280477</v>
+      </c>
+      <c r="G5">
+        <v>27199320</v>
+      </c>
+      <c r="H5">
+        <v>27176221</v>
+      </c>
+      <c r="I5">
+        <v>27153161</v>
+      </c>
+      <c r="J5">
+        <v>26722338</v>
+      </c>
+      <c r="K5">
+        <v>27245636</v>
+      </c>
+      <c r="L5">
+        <v>27257240</v>
+      </c>
+    </row>
+    <row r="6" spans="1:12">
+      <c r="A6">
+        <v>64</v>
+      </c>
+      <c r="B6">
+        <f t="shared" si="0"/>
+        <v>41.898527000000001</v>
+      </c>
+      <c r="C6">
+        <v>41898527</v>
+      </c>
+      <c r="D6">
+        <v>41816400</v>
+      </c>
+      <c r="E6">
+        <v>41816400</v>
+      </c>
+      <c r="F6">
+        <v>41789096</v>
+      </c>
+      <c r="G6">
+        <v>41303646</v>
+      </c>
+      <c r="H6">
+        <v>41707397</v>
+      </c>
+      <c r="I6">
+        <v>41518002</v>
+      </c>
+      <c r="J6">
+        <v>41898527</v>
+      </c>
+      <c r="K6">
+        <v>41734594</v>
+      </c>
+      <c r="L6">
+        <v>41357027</v>
+      </c>
+    </row>
+    <row r="7" spans="1:12">
+      <c r="A7">
+        <v>128</v>
+      </c>
+      <c r="B7">
+        <f t="shared" si="0"/>
+        <v>80.910240000000002</v>
+      </c>
+      <c r="C7">
+        <v>80629921</v>
+      </c>
+      <c r="D7">
+        <v>80680744</v>
+      </c>
+      <c r="E7">
+        <v>80477837</v>
+      </c>
+      <c r="F7">
+        <v>80528468</v>
+      </c>
+      <c r="G7">
+        <v>80808081</v>
+      </c>
+      <c r="H7">
+        <v>80757098</v>
+      </c>
+      <c r="I7">
+        <v>80757098</v>
+      </c>
+      <c r="J7">
+        <v>80553807</v>
+      </c>
+      <c r="K7">
+        <v>80833596</v>
+      </c>
+      <c r="L7">
+        <v>80910240</v>
+      </c>
+    </row>
+    <row r="8" spans="1:12">
+      <c r="A8">
+        <v>256</v>
+      </c>
+      <c r="B8">
+        <f t="shared" si="0"/>
+        <v>153.66146499999999</v>
+      </c>
+      <c r="C8">
+        <v>153523238</v>
+      </c>
+      <c r="D8">
+        <v>153431226</v>
+      </c>
+      <c r="E8">
+        <v>153431226</v>
+      </c>
+      <c r="F8">
+        <v>153523238</v>
+      </c>
+      <c r="G8">
+        <v>153569286</v>
+      </c>
+      <c r="H8">
+        <v>153339323</v>
+      </c>
+      <c r="I8">
+        <v>152790212</v>
+      </c>
+      <c r="J8">
+        <v>153431226</v>
+      </c>
+      <c r="K8">
+        <v>153155848</v>
+      </c>
+      <c r="L8">
+        <v>153661465</v>
+      </c>
+    </row>
+    <row r="9" spans="1:12">
+      <c r="A9">
+        <v>512</v>
+      </c>
+      <c r="B9">
+        <f t="shared" si="0"/>
+        <v>279.47598299999999</v>
+      </c>
+      <c r="C9">
+        <v>278412181</v>
+      </c>
+      <c r="D9">
+        <v>279171210</v>
+      </c>
+      <c r="E9">
+        <v>279475983</v>
+      </c>
+      <c r="F9">
+        <v>278639456</v>
+      </c>
+      <c r="G9">
+        <v>279323513</v>
+      </c>
+      <c r="H9">
+        <v>279323513</v>
+      </c>
+      <c r="I9">
+        <v>279475983</v>
+      </c>
+      <c r="J9">
+        <v>278715297</v>
+      </c>
+      <c r="K9">
+        <v>278867102</v>
+      </c>
+      <c r="L9">
+        <v>278943067</v>
+      </c>
+    </row>
+    <row r="10" spans="1:12">
+      <c r="A10">
+        <v>1024</v>
+      </c>
+      <c r="B10">
+        <f t="shared" si="0"/>
+        <v>482.56361900000002</v>
+      </c>
+      <c r="C10">
+        <v>482336317</v>
+      </c>
+      <c r="D10">
+        <v>482336317</v>
+      </c>
+      <c r="E10">
+        <v>478392899</v>
+      </c>
+      <c r="F10">
+        <v>481542441</v>
+      </c>
+      <c r="G10">
+        <v>480864053</v>
+      </c>
+      <c r="H10">
+        <v>479962503</v>
+      </c>
+      <c r="I10">
+        <v>481542441</v>
+      </c>
+      <c r="J10">
+        <v>481882353</v>
+      </c>
+      <c r="K10">
+        <v>480525575</v>
+      </c>
+      <c r="L10">
+        <v>482563619</v>
+      </c>
+    </row>
+    <row r="11" spans="1:12">
+      <c r="A11">
+        <v>2048</v>
+      </c>
+      <c r="B11">
+        <f t="shared" si="0"/>
+        <v>748.67483100000004</v>
+      </c>
+      <c r="C11">
+        <v>747172565</v>
+      </c>
+      <c r="D11">
+        <v>747718145</v>
+      </c>
+      <c r="E11">
+        <v>748401242</v>
+      </c>
+      <c r="F11">
+        <v>747172565</v>
+      </c>
+      <c r="G11">
+        <v>746219712</v>
+      </c>
+      <c r="H11">
+        <v>748127854</v>
+      </c>
+      <c r="I11">
+        <v>748674831</v>
+      </c>
+      <c r="J11">
+        <v>747308885</v>
+      </c>
+      <c r="K11">
+        <v>748538012</v>
+      </c>
+      <c r="L11">
+        <v>747991234</v>
+      </c>
+    </row>
+    <row r="12" spans="1:12">
+      <c r="A12">
+        <v>4096</v>
+      </c>
+      <c r="B12">
+        <f t="shared" si="0"/>
+        <v>1275.8137360000001</v>
+      </c>
+      <c r="C12">
+        <v>1275019455</v>
+      </c>
+      <c r="D12">
+        <v>1274821040</v>
+      </c>
+      <c r="E12">
+        <v>1275217933</v>
+      </c>
+      <c r="F12">
+        <v>1274622686</v>
+      </c>
+      <c r="G12">
+        <v>1275813736</v>
+      </c>
+      <c r="H12">
+        <v>1275416472</v>
+      </c>
+      <c r="I12">
+        <v>1274622686</v>
+      </c>
+      <c r="J12">
+        <v>1271062839</v>
+      </c>
+      <c r="K12">
+        <v>1275217933</v>
+      </c>
+      <c r="L12">
+        <v>1275217933</v>
+      </c>
+    </row>
+    <row r="13" spans="1:12">
+      <c r="A13">
+        <v>8192</v>
+      </c>
+      <c r="B13">
+        <f t="shared" si="0"/>
+        <v>1994.157741</v>
+      </c>
+      <c r="C13">
+        <v>1993429858</v>
+      </c>
+      <c r="D13">
+        <v>1994157741</v>
+      </c>
+      <c r="E13">
+        <v>1992944897</v>
+      </c>
+      <c r="F13">
+        <v>1993429858</v>
+      </c>
+      <c r="G13">
+        <v>1992702505</v>
+      </c>
+      <c r="H13">
+        <v>1990281827</v>
+      </c>
+      <c r="I13">
+        <v>1992702505</v>
+      </c>
+      <c r="J13">
+        <v>1994157741</v>
+      </c>
+      <c r="K13">
+        <v>1991491431</v>
+      </c>
+      <c r="L13">
+        <v>1993672426</v>
+      </c>
+    </row>
+    <row r="14" spans="1:12">
+      <c r="A14">
+        <v>16384</v>
+      </c>
+      <c r="B14">
+        <f t="shared" si="0"/>
+        <v>2795.9044370000001</v>
+      </c>
+      <c r="C14">
+        <v>2792568604</v>
+      </c>
+      <c r="D14">
+        <v>2792568604</v>
+      </c>
+      <c r="E14">
+        <v>2794950529</v>
+      </c>
+      <c r="F14">
+        <v>2794235525</v>
+      </c>
+      <c r="G14">
+        <v>2793759059</v>
+      </c>
+      <c r="H14">
+        <v>2795427401</v>
+      </c>
+      <c r="I14">
+        <v>2792568604</v>
+      </c>
+      <c r="J14">
+        <v>2793282755</v>
+      </c>
+      <c r="K14">
+        <v>2795904437</v>
+      </c>
+      <c r="L14">
+        <v>2795427401</v>
+      </c>
+    </row>
+    <row r="15" spans="1:12">
+      <c r="A15">
+        <v>32768</v>
+      </c>
+      <c r="B15">
+        <f t="shared" si="0"/>
+        <v>3492.0871740000002</v>
+      </c>
+      <c r="C15">
+        <v>3491343029</v>
+      </c>
+      <c r="D15">
+        <v>3490971075</v>
+      </c>
+      <c r="E15">
+        <v>3490227406</v>
+      </c>
+      <c r="F15">
+        <v>3488926746</v>
+      </c>
+      <c r="G15">
+        <v>3490599201</v>
+      </c>
+      <c r="H15">
+        <v>3491529036</v>
+      </c>
+      <c r="I15">
+        <v>3492087174</v>
+      </c>
+      <c r="J15">
+        <v>3491529036</v>
+      </c>
+      <c r="K15">
+        <v>3489669862</v>
+      </c>
+      <c r="L15">
+        <v>3492087174</v>
+      </c>
+    </row>
+    <row r="16" spans="1:12">
+      <c r="A16">
+        <v>65536</v>
+      </c>
+      <c r="B16">
+        <f t="shared" si="0"/>
+        <v>3997.9258810000001</v>
+      </c>
+      <c r="C16">
+        <v>3997438165</v>
+      </c>
+      <c r="D16">
+        <v>3997072457</v>
+      </c>
+      <c r="E16">
+        <v>3997560083</v>
+      </c>
+      <c r="F16">
+        <v>3997316255</v>
+      </c>
+      <c r="G16">
+        <v>3997438165</v>
+      </c>
+      <c r="H16">
+        <v>3997925881</v>
+      </c>
+      <c r="I16">
+        <v>3997072457</v>
+      </c>
+      <c r="J16">
+        <v>3997803941</v>
+      </c>
+      <c r="K16">
+        <v>3997682008</v>
+      </c>
+      <c r="L16">
+        <v>3997925881</v>
+      </c>
+    </row>
+    <row r="17" spans="1:12">
+      <c r="A17">
+        <v>131072</v>
+      </c>
+      <c r="B17">
+        <f t="shared" si="0"/>
+        <v>4314.275369</v>
+      </c>
+      <c r="C17">
+        <v>4313991377</v>
+      </c>
+      <c r="D17">
+        <v>4314062371</v>
+      </c>
+      <c r="E17">
+        <v>4313849394</v>
+      </c>
+      <c r="F17">
+        <v>4313991377</v>
+      </c>
+      <c r="G17">
+        <v>4313920384</v>
+      </c>
+      <c r="H17">
+        <v>4313778407</v>
+      </c>
+      <c r="I17">
+        <v>4314275369</v>
+      </c>
+      <c r="J17">
+        <v>4313920384</v>
+      </c>
+      <c r="K17">
+        <v>4313849394</v>
+      </c>
+      <c r="L17">
+        <v>4314204368</v>
+      </c>
+    </row>
+    <row r="18" spans="1:12">
+      <c r="A18">
+        <v>262144</v>
+      </c>
+      <c r="B18">
+        <f t="shared" si="0"/>
+        <v>4492.2286009999998</v>
+      </c>
+      <c r="C18">
+        <v>4492074644</v>
+      </c>
+      <c r="D18">
+        <v>4492228601</v>
+      </c>
+      <c r="E18">
+        <v>4491997670</v>
+      </c>
+      <c r="F18">
+        <v>4491959183</v>
+      </c>
+      <c r="G18">
+        <v>4492036156</v>
+      </c>
+      <c r="H18">
+        <v>4492036156</v>
+      </c>
+      <c r="I18">
+        <v>4492036156</v>
+      </c>
+      <c r="J18">
+        <v>4491728280</v>
+      </c>
+      <c r="K18">
+        <v>4492074644</v>
+      </c>
+      <c r="L18">
+        <v>4492190111</v>
+      </c>
+    </row>
+    <row r="19" spans="1:12">
+      <c r="A19">
+        <v>524288</v>
+      </c>
+      <c r="B19">
+        <f t="shared" si="0"/>
+        <v>4586.6657340000002</v>
+      </c>
+      <c r="C19">
+        <v>4586525297</v>
+      </c>
+      <c r="D19">
+        <v>4586665734</v>
+      </c>
+      <c r="E19">
+        <v>4586505236</v>
+      </c>
+      <c r="F19">
+        <v>4586505236</v>
+      </c>
+      <c r="G19">
+        <v>4586404930</v>
+      </c>
+      <c r="H19">
+        <v>4586545359</v>
+      </c>
+      <c r="I19">
+        <v>4586605546</v>
+      </c>
+      <c r="J19">
+        <v>4586545359</v>
+      </c>
+      <c r="K19">
+        <v>4586485174</v>
+      </c>
+      <c r="L19">
+        <v>4586585483</v>
+      </c>
+    </row>
+    <row r="20" spans="1:12">
+      <c r="A20">
+        <v>1048576</v>
+      </c>
+      <c r="B20">
+        <f t="shared" si="0"/>
+        <v>4636.2806330000003</v>
+      </c>
+      <c r="C20">
+        <v>4636219136</v>
+      </c>
+      <c r="D20">
+        <v>4636260133</v>
+      </c>
+      <c r="E20">
+        <v>4636249884</v>
+      </c>
+      <c r="F20">
+        <v>4636239634</v>
+      </c>
+      <c r="G20">
+        <v>4636270383</v>
+      </c>
+      <c r="H20">
+        <v>4636208886</v>
+      </c>
+      <c r="I20">
+        <v>4636280633</v>
+      </c>
+      <c r="J20">
+        <v>4636260133</v>
+      </c>
+      <c r="K20">
+        <v>4636270383</v>
+      </c>
+      <c r="L20">
+        <v>4636280633</v>
+      </c>
+    </row>
+    <row r="21" spans="1:12">
+      <c r="A21">
+        <v>2097152</v>
+      </c>
+      <c r="B21">
+        <f t="shared" si="0"/>
+        <v>4661.6844869999995</v>
+      </c>
+      <c r="C21">
+        <v>4661648219</v>
+      </c>
+      <c r="D21">
+        <v>4661674124</v>
+      </c>
+      <c r="E21">
+        <v>4661663762</v>
+      </c>
+      <c r="F21">
+        <v>4661658581</v>
+      </c>
+      <c r="G21">
+        <v>4661679305</v>
+      </c>
+      <c r="H21">
+        <v>4661648219</v>
+      </c>
+      <c r="I21">
+        <v>4661663762</v>
+      </c>
+      <c r="J21">
+        <v>4661684487</v>
+      </c>
+      <c r="K21">
+        <v>4661653400</v>
+      </c>
+      <c r="L21">
+        <v>4661648219</v>
+      </c>
+    </row>
+    <row r="22" spans="1:12">
+      <c r="A22">
+        <v>4194304</v>
+      </c>
+      <c r="B22">
+        <f t="shared" si="0"/>
+        <v>4674.5093320000005</v>
+      </c>
+      <c r="C22">
+        <v>4674496308</v>
+      </c>
+      <c r="D22">
+        <v>4674498913</v>
+      </c>
+      <c r="E22">
+        <v>4674491098</v>
+      </c>
+      <c r="F22">
+        <v>4674496308</v>
+      </c>
+      <c r="G22">
+        <v>4674493703</v>
+      </c>
+      <c r="H22">
+        <v>4674496308</v>
+      </c>
+      <c r="I22">
+        <v>4674496308</v>
+      </c>
+      <c r="J22">
+        <v>4674509332</v>
+      </c>
+      <c r="K22">
+        <v>4674496308</v>
+      </c>
+      <c r="L22">
+        <v>4674498913</v>
+      </c>
+    </row>
+    <row r="23" spans="1:12">
+      <c r="A23">
+        <v>8388608</v>
+      </c>
+      <c r="B23">
+        <f t="shared" si="0"/>
+        <v>4680.9560889999993</v>
+      </c>
+      <c r="C23">
+        <v>4680944335</v>
+      </c>
+      <c r="D23">
+        <v>4680950865</v>
+      </c>
+      <c r="E23">
+        <v>4680946947</v>
+      </c>
+      <c r="F23">
+        <v>4680945641</v>
+      </c>
+      <c r="G23">
+        <v>4680945641</v>
+      </c>
+      <c r="H23">
+        <v>4680944335</v>
+      </c>
+      <c r="I23">
+        <v>4680956089</v>
+      </c>
+      <c r="J23">
+        <v>4680949559</v>
+      </c>
+      <c r="K23">
+        <v>4680952171</v>
+      </c>
+      <c r="L23">
+        <v>4680954783</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="1"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:L23"/>
+  <sheetViews>
+    <sheetView showRuler="0" workbookViewId="0">
+      <selection activeCell="L2" sqref="L2:L23"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="12" defaultRowHeight="18" x14ac:dyDescent="0"/>
+  <sheetData>
+    <row r="1" spans="1:12">
+      <c r="A1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1">
+        <v>1</v>
+      </c>
+      <c r="D1">
+        <v>2</v>
+      </c>
+      <c r="E1">
+        <v>3</v>
+      </c>
+      <c r="F1">
+        <v>4</v>
+      </c>
+      <c r="G1">
+        <v>5</v>
+      </c>
+      <c r="H1">
+        <v>6</v>
+      </c>
+      <c r="I1">
+        <v>7</v>
+      </c>
+      <c r="J1">
+        <v>8</v>
+      </c>
+      <c r="K1">
+        <v>9</v>
+      </c>
+      <c r="L1">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="2" spans="1:12">
+      <c r="A2">
+        <v>4</v>
+      </c>
+      <c r="B2">
+        <f t="shared" ref="B2:B23" si="0">MAX(C2:L2)/1000/1000</f>
+        <v>0.72833199999999998</v>
+      </c>
+      <c r="C2">
+        <v>728200</v>
+      </c>
+      <c r="D2">
+        <v>726678</v>
+      </c>
+      <c r="E2">
+        <v>723066</v>
+      </c>
+      <c r="F2">
+        <v>726414</v>
+      </c>
+      <c r="G2">
+        <v>727736</v>
+      </c>
+      <c r="H2">
+        <v>726085</v>
+      </c>
+      <c r="I2">
+        <v>726216</v>
+      </c>
+      <c r="J2">
+        <v>725821</v>
+      </c>
+      <c r="K2">
+        <v>720916</v>
+      </c>
+      <c r="L2">
+        <v>728332</v>
+      </c>
+    </row>
+    <row r="3" spans="1:12">
+      <c r="A3">
+        <v>8</v>
+      </c>
+      <c r="B3">
+        <f t="shared" si="0"/>
+        <v>1.4329210000000001</v>
+      </c>
+      <c r="C3">
+        <v>1425898</v>
+      </c>
+      <c r="D3">
+        <v>1392879</v>
+      </c>
+      <c r="E3">
+        <v>1430359</v>
+      </c>
+      <c r="F3">
+        <v>1432921</v>
+      </c>
+      <c r="G3">
+        <v>1425771</v>
+      </c>
+      <c r="H3">
+        <v>1410686</v>
+      </c>
+      <c r="I3">
+        <v>1428571</v>
+      </c>
+      <c r="J3">
+        <v>1428699</v>
+      </c>
+      <c r="K3">
+        <v>1430487</v>
+      </c>
+      <c r="L3">
+        <v>1429337</v>
+      </c>
+    </row>
+    <row r="4" spans="1:12">
+      <c r="A4">
+        <v>16</v>
+      </c>
+      <c r="B4">
+        <f t="shared" si="0"/>
+        <v>2.978129</v>
+      </c>
+      <c r="C4">
+        <v>2973149</v>
+      </c>
+      <c r="D4">
+        <v>2977852</v>
+      </c>
+      <c r="E4">
+        <v>2976744</v>
+      </c>
+      <c r="F4">
+        <v>2971216</v>
+      </c>
+      <c r="G4">
+        <v>2975914</v>
+      </c>
+      <c r="H4">
+        <v>2972044</v>
+      </c>
+      <c r="I4">
+        <v>2969286</v>
+      </c>
+      <c r="J4">
+        <v>2971492</v>
+      </c>
+      <c r="K4">
+        <v>2978129</v>
+      </c>
+      <c r="L4">
+        <v>2971768</v>
+      </c>
+    </row>
+    <row r="5" spans="1:12">
+      <c r="A5">
+        <v>32</v>
+      </c>
+      <c r="B5">
+        <f t="shared" si="0"/>
+        <v>5.9869040000000009</v>
+      </c>
+      <c r="C5">
+        <v>5977398</v>
+      </c>
+      <c r="D5">
+        <v>5977398</v>
+      </c>
+      <c r="E5">
+        <v>5974608</v>
+      </c>
+      <c r="F5">
+        <v>5976282</v>
+      </c>
+      <c r="G5">
+        <v>5986904</v>
+      </c>
+      <c r="H5">
+        <v>5979632</v>
+      </c>
+      <c r="I5">
+        <v>5972378</v>
+      </c>
+      <c r="J5">
+        <v>5984664</v>
+      </c>
+      <c r="K5">
+        <v>5981867</v>
+      </c>
+      <c r="L5">
+        <v>5981867</v>
+      </c>
+    </row>
+    <row r="6" spans="1:12">
+      <c r="A6">
+        <v>64</v>
+      </c>
+      <c r="B6">
+        <f t="shared" si="0"/>
+        <v>11.962617</v>
+      </c>
+      <c r="C6">
+        <v>11946985</v>
+      </c>
+      <c r="D6">
+        <v>11955913</v>
+      </c>
+      <c r="E6">
+        <v>11945870</v>
+      </c>
+      <c r="F6">
+        <v>11953679</v>
+      </c>
+      <c r="G6">
+        <v>11962617</v>
+      </c>
+      <c r="H6">
+        <v>11953679</v>
+      </c>
+      <c r="I6">
+        <v>11960381</v>
+      </c>
+      <c r="J6">
+        <v>11953679</v>
+      </c>
+      <c r="K6">
+        <v>11952563</v>
+      </c>
+      <c r="L6">
+        <v>11961499</v>
+      </c>
+    </row>
+    <row r="7" spans="1:12">
+      <c r="A7">
+        <v>128</v>
+      </c>
+      <c r="B7">
+        <f t="shared" si="0"/>
+        <v>24.162341000000001</v>
+      </c>
+      <c r="C7">
+        <v>24112273</v>
+      </c>
+      <c r="D7">
+        <v>24128181</v>
+      </c>
+      <c r="E7">
+        <v>24141833</v>
+      </c>
+      <c r="F7">
+        <v>24148665</v>
+      </c>
+      <c r="G7">
+        <v>24162341</v>
+      </c>
+      <c r="H7">
+        <v>24137281</v>
+      </c>
+      <c r="I7">
+        <v>24123634</v>
+      </c>
+      <c r="J7">
+        <v>24125907</v>
+      </c>
+      <c r="K7">
+        <v>24144110</v>
+      </c>
+      <c r="L7">
+        <v>24121361</v>
+      </c>
+    </row>
+    <row r="8" spans="1:12">
+      <c r="A8">
+        <v>256</v>
+      </c>
+      <c r="B8">
+        <f t="shared" si="0"/>
+        <v>47.132468000000003</v>
+      </c>
+      <c r="C8">
+        <v>47110784</v>
+      </c>
+      <c r="D8">
+        <v>46255308</v>
+      </c>
+      <c r="E8">
+        <v>47054499</v>
+      </c>
+      <c r="F8">
+        <v>47123792</v>
+      </c>
+      <c r="G8">
+        <v>46890741</v>
+      </c>
+      <c r="H8">
+        <v>46920821</v>
+      </c>
+      <c r="I8">
+        <v>47132468</v>
+      </c>
+      <c r="J8">
+        <v>47089120</v>
+      </c>
+      <c r="K8">
+        <v>47089120</v>
+      </c>
+      <c r="L8">
+        <v>47123792</v>
+      </c>
+    </row>
+    <row r="9" spans="1:12">
+      <c r="A9">
+        <v>512</v>
+      </c>
+      <c r="B9">
+        <f t="shared" si="0"/>
+        <v>94.247584000000003</v>
+      </c>
+      <c r="C9">
+        <v>93936336</v>
+      </c>
+      <c r="D9">
+        <v>94152262</v>
+      </c>
+      <c r="E9">
+        <v>94186902</v>
+      </c>
+      <c r="F9">
+        <v>94195566</v>
+      </c>
+      <c r="G9">
+        <v>94238910</v>
+      </c>
+      <c r="H9">
+        <v>94143606</v>
+      </c>
+      <c r="I9">
+        <v>94186902</v>
+      </c>
+      <c r="J9">
+        <v>94247584</v>
+      </c>
+      <c r="K9">
+        <v>94126298</v>
+      </c>
+      <c r="L9">
+        <v>94230238</v>
+      </c>
+    </row>
+    <row r="10" spans="1:12">
+      <c r="A10">
+        <v>1024</v>
+      </c>
+      <c r="B10">
+        <f t="shared" si="0"/>
+        <v>184.089888</v>
+      </c>
+      <c r="C10">
+        <v>183908046</v>
+      </c>
+      <c r="D10">
+        <v>183908046</v>
+      </c>
+      <c r="E10">
+        <v>184007188</v>
+      </c>
+      <c r="F10">
+        <v>183891533</v>
+      </c>
+      <c r="G10">
+        <v>184089888</v>
+      </c>
+      <c r="H10">
+        <v>183924562</v>
+      </c>
+      <c r="I10">
+        <v>183858515</v>
+      </c>
+      <c r="J10">
+        <v>183809011</v>
+      </c>
+      <c r="K10">
+        <v>183941081</v>
+      </c>
+      <c r="L10">
+        <v>184023722</v>
+      </c>
+    </row>
+    <row r="11" spans="1:12">
+      <c r="A11">
+        <v>2048</v>
+      </c>
+      <c r="B11">
+        <f t="shared" si="0"/>
+        <v>350.83511800000002</v>
+      </c>
+      <c r="C11">
+        <v>350624893</v>
+      </c>
+      <c r="D11">
+        <v>350504878</v>
+      </c>
+      <c r="E11">
+        <v>350714958</v>
+      </c>
+      <c r="F11">
+        <v>350564875</v>
+      </c>
+      <c r="G11">
+        <v>350504878</v>
+      </c>
+      <c r="H11">
+        <v>350354974</v>
+      </c>
+      <c r="I11">
+        <v>350744991</v>
+      </c>
+      <c r="J11">
+        <v>350564875</v>
+      </c>
+      <c r="K11">
+        <v>350805070</v>
+      </c>
+      <c r="L11">
+        <v>350835118</v>
+      </c>
+    </row>
+    <row r="12" spans="1:12">
+      <c r="A12">
+        <v>4096</v>
+      </c>
+      <c r="B12">
+        <f t="shared" si="0"/>
+        <v>663.319838</v>
+      </c>
+      <c r="C12">
+        <v>662300914</v>
+      </c>
+      <c r="D12">
+        <v>662247373</v>
+      </c>
+      <c r="E12">
+        <v>662622341</v>
+      </c>
+      <c r="F12">
+        <v>662729553</v>
+      </c>
+      <c r="G12">
+        <v>662354463</v>
+      </c>
+      <c r="H12">
+        <v>663051396</v>
+      </c>
+      <c r="I12">
+        <v>661498708</v>
+      </c>
+      <c r="J12">
+        <v>663319838</v>
+      </c>
+      <c r="K12">
+        <v>662783172</v>
+      </c>
+      <c r="L12">
+        <v>662354463</v>
+      </c>
+    </row>
+    <row r="13" spans="1:12">
+      <c r="A13">
+        <v>8192</v>
+      </c>
+      <c r="B13">
+        <f t="shared" si="0"/>
+        <v>1168.782993</v>
+      </c>
+      <c r="C13">
+        <v>1166785358</v>
+      </c>
+      <c r="D13">
+        <v>1167783321</v>
+      </c>
+      <c r="E13">
+        <v>1167700093</v>
+      </c>
+      <c r="F13">
+        <v>1166453083</v>
+      </c>
+      <c r="G13">
+        <v>1167284127</v>
+      </c>
+      <c r="H13">
+        <v>1166951567</v>
+      </c>
+      <c r="I13">
+        <v>1166868457</v>
+      </c>
+      <c r="J13">
+        <v>1168782993</v>
+      </c>
+      <c r="K13">
+        <v>1167616876</v>
+      </c>
+      <c r="L13">
+        <v>1167949815</v>
+      </c>
+    </row>
+    <row r="14" spans="1:12">
+      <c r="A14">
+        <v>16384</v>
+      </c>
+      <c r="B14">
+        <f t="shared" si="0"/>
+        <v>1876.961851</v>
+      </c>
+      <c r="C14">
+        <v>1875565222</v>
+      </c>
+      <c r="D14">
+        <v>1875457875</v>
+      </c>
+      <c r="E14">
+        <v>1875243218</v>
+      </c>
+      <c r="F14">
+        <v>1875887337</v>
+      </c>
+      <c r="G14">
+        <v>1876961851</v>
+      </c>
+      <c r="H14">
+        <v>1876209562</v>
+      </c>
+      <c r="I14">
+        <v>1875887337</v>
+      </c>
+      <c r="J14">
+        <v>1876209562</v>
+      </c>
+      <c r="K14">
+        <v>1875457875</v>
+      </c>
+      <c r="L14">
+        <v>1875994733</v>
+      </c>
+    </row>
+    <row r="15" spans="1:12">
+      <c r="A15">
+        <v>32768</v>
+      </c>
+      <c r="B15">
+        <f t="shared" si="0"/>
+        <v>2690.7538180000001</v>
+      </c>
+      <c r="C15">
+        <v>2687553824</v>
+      </c>
+      <c r="D15">
+        <v>2686892706</v>
+      </c>
+      <c r="E15">
+        <v>2689318396</v>
+      </c>
+      <c r="F15">
+        <v>2687223225</v>
+      </c>
+      <c r="G15">
+        <v>2689870300</v>
+      </c>
+      <c r="H15">
+        <v>2688215267</v>
+      </c>
+      <c r="I15">
+        <v>2689980708</v>
+      </c>
+      <c r="J15">
+        <v>2689318396</v>
+      </c>
+      <c r="K15">
+        <v>2689539131</v>
+      </c>
+      <c r="L15">
+        <v>2690753818</v>
+      </c>
+    </row>
+    <row r="16" spans="1:12">
+      <c r="A16">
+        <v>65536</v>
+      </c>
+      <c r="B16">
+        <f t="shared" si="0"/>
+        <v>3437.9540980000002</v>
+      </c>
+      <c r="C16">
+        <v>3437052576</v>
+      </c>
+      <c r="D16">
+        <v>3436692100</v>
+      </c>
+      <c r="E16">
+        <v>3437593433</v>
+      </c>
+      <c r="F16">
+        <v>3437593433</v>
+      </c>
+      <c r="G16">
+        <v>3436962450</v>
+      </c>
+      <c r="H16">
+        <v>3437954098</v>
+      </c>
+      <c r="I16">
+        <v>3437052576</v>
+      </c>
+      <c r="J16">
+        <v>3436241611</v>
+      </c>
+      <c r="K16">
+        <v>3436782212</v>
+      </c>
+      <c r="L16">
+        <v>3437503278</v>
+      </c>
+    </row>
+    <row r="17" spans="1:12">
+      <c r="A17">
+        <v>131072</v>
+      </c>
+      <c r="B17">
+        <f t="shared" si="0"/>
+        <v>3993.4798839999999</v>
+      </c>
+      <c r="C17">
+        <v>3992932432</v>
+      </c>
+      <c r="D17">
+        <v>3992993252</v>
+      </c>
+      <c r="E17">
+        <v>3993479884</v>
+      </c>
+      <c r="F17">
+        <v>3993114899</v>
+      </c>
+      <c r="G17">
+        <v>3992445934</v>
+      </c>
+      <c r="H17">
+        <v>3993297383</v>
+      </c>
+      <c r="I17">
+        <v>3993236553</v>
+      </c>
+      <c r="J17">
+        <v>3993479884</v>
+      </c>
+      <c r="K17">
+        <v>3993479884</v>
+      </c>
+      <c r="L17">
+        <v>3993479884</v>
+      </c>
+    </row>
+    <row r="18" spans="1:12">
+      <c r="A18">
+        <v>262144</v>
+      </c>
+      <c r="B18">
+        <f t="shared" si="0"/>
+        <v>4343.4763519999997</v>
+      </c>
+      <c r="C18">
+        <v>4343476352</v>
+      </c>
+      <c r="D18">
+        <v>4343188502</v>
+      </c>
+      <c r="E18">
+        <v>4342612916</v>
+      </c>
+      <c r="F18">
+        <v>4343152523</v>
+      </c>
+      <c r="G18">
+        <v>4343080568</v>
+      </c>
+      <c r="H18">
+        <v>4343368404</v>
+      </c>
+      <c r="I18">
+        <v>4342936664</v>
+      </c>
+      <c r="J18">
+        <v>4343476352</v>
+      </c>
+      <c r="K18">
+        <v>4343368404</v>
+      </c>
+      <c r="L18">
+        <v>4343332422</v>
+      </c>
+    </row>
+    <row r="19" spans="1:12">
+      <c r="A19">
+        <v>524288</v>
+      </c>
+      <c r="B19">
+        <f t="shared" si="0"/>
+        <v>4541.2166200000001</v>
+      </c>
+      <c r="C19">
+        <v>4540154835</v>
+      </c>
+      <c r="D19">
+        <v>4540980625</v>
+      </c>
+      <c r="E19">
+        <v>4540371084</v>
+      </c>
+      <c r="F19">
+        <v>4540017232</v>
+      </c>
+      <c r="G19">
+        <v>4540548031</v>
+      </c>
+      <c r="H19">
+        <v>4541216620</v>
+      </c>
+      <c r="I19">
+        <v>4540194151</v>
+      </c>
+      <c r="J19">
+        <v>4540449725</v>
+      </c>
+      <c r="K19">
+        <v>4540312105</v>
+      </c>
+      <c r="L19">
+        <v>4540154835</v>
+      </c>
+    </row>
+    <row r="20" spans="1:12">
+      <c r="A20">
+        <v>1048576</v>
+      </c>
+      <c r="B20">
+        <f t="shared" si="0"/>
+        <v>4649.2518949999994</v>
+      </c>
+      <c r="C20">
+        <v>4648963314</v>
+      </c>
+      <c r="D20">
+        <v>4649076681</v>
+      </c>
+      <c r="E20">
+        <v>4649251895</v>
+      </c>
+      <c r="F20">
+        <v>4649086987</v>
+      </c>
+      <c r="G20">
+        <v>4649220974</v>
+      </c>
+      <c r="H20">
+        <v>4648973620</v>
+      </c>
+      <c r="I20">
+        <v>4649056068</v>
+      </c>
+      <c r="J20">
+        <v>4649056068</v>
+      </c>
+      <c r="K20">
+        <v>4649179746</v>
+      </c>
+      <c r="L20">
+        <v>4648973620</v>
+      </c>
+    </row>
+    <row r="21" spans="1:12">
+      <c r="A21">
+        <v>2097152</v>
+      </c>
+      <c r="B21">
+        <f t="shared" si="0"/>
+        <v>4704.1912940000002</v>
+      </c>
+      <c r="C21">
+        <v>4703969710</v>
+      </c>
+      <c r="D21">
+        <v>4703885303</v>
+      </c>
+      <c r="E21">
+        <v>4703880027</v>
+      </c>
+      <c r="F21">
+        <v>4703938057</v>
+      </c>
+      <c r="G21">
+        <v>4703938057</v>
+      </c>
+      <c r="H21">
+        <v>4704191294</v>
+      </c>
+      <c r="I21">
+        <v>4703858926</v>
+      </c>
+      <c r="J21">
+        <v>4704027742</v>
+      </c>
+      <c r="K21">
+        <v>4703974986</v>
+      </c>
+      <c r="L21">
+        <v>4703943332</v>
+      </c>
+    </row>
+    <row r="22" spans="1:12">
+      <c r="A22">
+        <v>4194304</v>
+      </c>
+      <c r="B22">
+        <f t="shared" si="0"/>
+        <v>4732.852973</v>
+      </c>
+      <c r="C22">
+        <v>4732823601</v>
+      </c>
+      <c r="D22">
+        <v>4732540572</v>
+      </c>
+      <c r="E22">
+        <v>4732844963</v>
+      </c>
+      <c r="F22">
+        <v>4732818260</v>
+      </c>
+      <c r="G22">
+        <v>4732842292</v>
+      </c>
+      <c r="H22">
+        <v>4732548582</v>
+      </c>
+      <c r="I22">
+        <v>4732815590</v>
+      </c>
+      <c r="J22">
+        <v>4732836952</v>
+      </c>
+      <c r="K22">
+        <v>4732844963</v>
+      </c>
+      <c r="L22">
+        <v>4732852973</v>
+      </c>
+    </row>
+    <row r="23" spans="1:12">
+      <c r="A23">
+        <v>8388608</v>
+      </c>
+      <c r="B23">
+        <f t="shared" si="0"/>
+        <v>4746.8544749999992</v>
+      </c>
+      <c r="C23">
+        <v>4746736289</v>
+      </c>
+      <c r="D23">
+        <v>4746849103</v>
+      </c>
+      <c r="E23">
+        <v>4746710773</v>
+      </c>
+      <c r="F23">
+        <v>4746675856</v>
+      </c>
+      <c r="G23">
+        <v>4746733604</v>
+      </c>
+      <c r="H23">
+        <v>4746854475</v>
+      </c>
+      <c r="I23">
+        <v>4746720174</v>
+      </c>
+      <c r="J23">
+        <v>4746730918</v>
+      </c>
+      <c r="K23">
+        <v>4746717488</v>
+      </c>
+      <c r="L23">
+        <v>4746751062</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="1"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
+</worksheet>
 </file>
</xml_diff>